<commit_message>
MAJOR : adaptations of soil model for separated, and possibly autonomous, execution
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios_24-09-13.xlsx
+++ b/test/inputs/Scenarios_24-09-13.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\simulations\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\simulations\single_plant\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040B088-EA4F-468F-B08C-A5BADD44213C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE445D9-C397-4BA2-99C6-349A40DA0401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="564">
   <si>
     <t>input_file</t>
   </si>
@@ -1500,18 +1500,12 @@
     <t>adim</t>
   </si>
   <si>
-    <t>C_mineralN_soil</t>
-  </si>
-  <si>
     <t>Mean soil concentration in nitrates</t>
   </si>
   <si>
     <t>mol.m-3</t>
   </si>
   <si>
-    <t>water_potential_soil</t>
-  </si>
-  <si>
     <t>Mean soil water potential</t>
   </si>
   <si>
@@ -1524,9 +1518,6 @@
     <t>xylem uniform pressure</t>
   </si>
   <si>
-    <t>C_mineralN_patch</t>
-  </si>
-  <si>
     <t>Mineral nitrogen concentration in a located patch in soil</t>
   </si>
   <si>
@@ -1693,6 +1684,48 @@
   </si>
   <si>
     <t>WB8</t>
+  </si>
+  <si>
+    <t>water_moisture_patch</t>
+  </si>
+  <si>
+    <t>root_cynaps</t>
+  </si>
+  <si>
+    <t>water moisture in a located patch in soil</t>
+  </si>
+  <si>
+    <t>patch_depth_water_moisture</t>
+  </si>
+  <si>
+    <t>Depth of a water moisture patch in soil</t>
+  </si>
+  <si>
+    <t>patch_uniform_width_water_moisture</t>
+  </si>
+  <si>
+    <t>Width of the zone of the patch with uniform water moisture</t>
+  </si>
+  <si>
+    <t>patch_transition_water_moisture</t>
+  </si>
+  <si>
+    <t>Variance of the normal law smooting the boundary transition of a moisture patch with the background concentration</t>
+  </si>
+  <si>
+    <t>smax_AA</t>
+  </si>
+  <si>
+    <t>Maximal rate of amino acid synthesis in the root segment</t>
+  </si>
+  <si>
+    <t>content_mineralN_soil</t>
+  </si>
+  <si>
+    <t>soil_moisture</t>
+  </si>
+  <si>
+    <t>content_mineralN_patch</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -2299,6 +2332,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2344,7 +2390,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2413,50 +2459,66 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="16" fillId="51" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2734,16 +2796,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z222"/>
+  <dimension ref="A1:AO227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="J42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G195" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
@@ -2779,37 +2841,37 @@
         <v>378</v>
       </c>
       <c r="H1" s="35" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J1" s="36" t="s">
+        <v>541</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>543</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>544</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="M1" s="36" t="s">
+        <v>542</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>545</v>
+      </c>
+      <c r="O1" s="36" t="s">
         <v>546</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>547</v>
       </c>
-      <c r="M1" s="36" t="s">
-        <v>545</v>
-      </c>
-      <c r="N1" s="36" t="s">
+      <c r="Q1" s="36" t="s">
         <v>548</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="R1" s="36" t="s">
         <v>549</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>550</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>551</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2823,7 +2885,7 @@
         <v>483</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E2" s="43" t="s">
         <v>447</v>
@@ -2880,7 +2942,7 @@
         <v>483</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E3" s="46" t="s">
         <v>477</v>
@@ -2936,7 +2998,7 @@
         <v>483</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>129</v>
@@ -2993,7 +3055,7 @@
         <v>483</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>130</v>
@@ -3050,7 +3112,7 @@
         <v>483</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>114</v>
@@ -3107,7 +3169,7 @@
         <v>483</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>115</v>
@@ -3164,7 +3226,7 @@
         <v>483</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>123</v>
@@ -3221,7 +3283,7 @@
         <v>483</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>113</v>
@@ -3278,7 +3340,7 @@
         <v>483</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>451</v>
@@ -3335,7 +3397,7 @@
         <v>483</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>131</v>
@@ -3392,7 +3454,7 @@
         <v>483</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>116</v>
@@ -3449,7 +3511,7 @@
         <v>483</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>117</v>
@@ -3506,7 +3568,7 @@
         <v>483</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>458</v>
@@ -3563,7 +3625,7 @@
         <v>483</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>465</v>
@@ -3620,7 +3682,7 @@
         <v>483</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>468</v>
@@ -3677,7 +3739,7 @@
         <v>483</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>470</v>
@@ -3734,7 +3796,7 @@
         <v>483</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>133</v>
@@ -3790,7 +3852,7 @@
         <v>483</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>118</v>
@@ -3847,7 +3909,7 @@
         <v>483</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>363</v>
@@ -3904,7 +3966,7 @@
         <v>483</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>365</v>
@@ -3961,7 +4023,7 @@
         <v>483</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>377</v>
@@ -4018,7 +4080,7 @@
         <v>483</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>373</v>
@@ -4075,7 +4137,7 @@
         <v>483</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>372</v>
@@ -4132,7 +4194,7 @@
         <v>483</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>139</v>
@@ -4189,7 +4251,7 @@
         <v>483</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>119</v>
@@ -4246,7 +4308,7 @@
         <v>483</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>134</v>
@@ -4303,7 +4365,7 @@
         <v>483</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>132</v>
@@ -4360,7 +4422,7 @@
         <v>483</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>457</v>
@@ -4417,7 +4479,7 @@
         <v>483</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>137</v>
@@ -4474,7 +4536,7 @@
         <v>483</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>124</v>
@@ -4531,7 +4593,7 @@
         <v>483</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>125</v>
@@ -4588,7 +4650,7 @@
         <v>483</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>126</v>
@@ -4645,7 +4707,7 @@
         <v>483</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>138</v>
@@ -4702,7 +4764,7 @@
         <v>483</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>127</v>
@@ -4759,7 +4821,7 @@
         <v>483</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>128</v>
@@ -4816,7 +4878,7 @@
         <v>483</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>140</v>
@@ -4873,7 +4935,7 @@
         <v>483</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>141</v>
@@ -4930,7 +4992,7 @@
         <v>483</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>142</v>
@@ -4987,7 +5049,7 @@
         <v>483</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>143</v>
@@ -5044,7 +5106,7 @@
         <v>483</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>144</v>
@@ -5101,7 +5163,7 @@
         <v>483</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>145</v>
@@ -5158,7 +5220,7 @@
         <v>483</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>146</v>
@@ -5215,7 +5277,7 @@
         <v>483</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>147</v>
@@ -5272,7 +5334,7 @@
         <v>483</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>439</v>
@@ -5329,7 +5391,7 @@
         <v>483</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>440</v>
@@ -5386,7 +5448,7 @@
         <v>483</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>460</v>
@@ -5443,7 +5505,7 @@
         <v>483</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>135</v>
@@ -5500,7 +5562,7 @@
         <v>483</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>136</v>
@@ -5557,7 +5619,7 @@
         <v>483</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>120</v>
@@ -5614,7 +5676,7 @@
         <v>483</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>121</v>
@@ -5671,7 +5733,7 @@
         <v>483</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>122</v>
@@ -5728,7 +5790,7 @@
         <v>483</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E53" s="16" t="s">
         <v>148</v>
@@ -5785,7 +5847,7 @@
         <v>483</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>380</v>
@@ -5842,7 +5904,7 @@
         <v>483</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>149</v>
@@ -5899,7 +5961,7 @@
         <v>483</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>150</v>
@@ -5956,7 +6018,7 @@
         <v>483</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E57" s="18" t="s">
         <v>151</v>
@@ -6013,7 +6075,7 @@
         <v>483</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E58" s="18" t="s">
         <v>152</v>
@@ -6070,7 +6132,7 @@
         <v>483</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E59" s="18" t="s">
         <v>284</v>
@@ -6127,7 +6189,7 @@
         <v>483</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E60" s="18" t="s">
         <v>155</v>
@@ -6184,7 +6246,7 @@
         <v>483</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E61" s="18" t="s">
         <v>407</v>
@@ -6241,7 +6303,7 @@
         <v>483</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>153</v>
@@ -6298,7 +6360,7 @@
         <v>483</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>409</v>
@@ -6355,7 +6417,7 @@
         <v>483</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>154</v>
@@ -6412,7 +6474,7 @@
         <v>483</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>288</v>
@@ -6469,7 +6531,7 @@
         <v>483</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>381</v>
@@ -6526,7 +6588,7 @@
         <v>483</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>156</v>
@@ -6583,7 +6645,7 @@
         <v>483</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>157</v>
@@ -6640,7 +6702,7 @@
         <v>483</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>158</v>
@@ -6697,7 +6759,7 @@
         <v>483</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>159</v>
@@ -6754,7 +6816,7 @@
         <v>483</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>160</v>
@@ -6811,7 +6873,7 @@
         <v>483</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>161</v>
@@ -6868,7 +6930,7 @@
         <v>483</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E73" s="34" t="s">
         <v>419</v>
@@ -6925,7 +6987,7 @@
         <v>483</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E74" s="34" t="s">
         <v>413</v>
@@ -6982,7 +7044,7 @@
         <v>483</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E75" s="34" t="s">
         <v>420</v>
@@ -7039,7 +7101,7 @@
         <v>483</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E76" s="34" t="s">
         <v>403</v>
@@ -7096,7 +7158,7 @@
         <v>483</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E77" s="34" t="s">
         <v>416</v>
@@ -7153,7 +7215,7 @@
         <v>483</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E78" s="34" t="s">
         <v>415</v>
@@ -7210,7 +7272,7 @@
         <v>483</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>417</v>
@@ -7267,7 +7329,7 @@
         <v>483</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>404</v>
@@ -7324,7 +7386,7 @@
         <v>483</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>405</v>
@@ -7381,7 +7443,7 @@
         <v>483</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E82" s="18" t="s">
         <v>162</v>
@@ -7438,7 +7500,7 @@
         <v>483</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E83" s="18" t="s">
         <v>163</v>
@@ -7495,7 +7557,7 @@
         <v>483</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E84" s="18" t="s">
         <v>164</v>
@@ -7552,7 +7614,7 @@
         <v>483</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E85" s="18" t="s">
         <v>165</v>
@@ -7609,7 +7671,7 @@
         <v>483</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E86" s="18" t="s">
         <v>166</v>
@@ -7666,7 +7728,7 @@
         <v>483</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E87" s="20" t="s">
         <v>290</v>
@@ -7723,7 +7785,7 @@
         <v>483</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>291</v>
@@ -7780,7 +7842,7 @@
         <v>483</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>295</v>
@@ -7837,7 +7899,7 @@
         <v>483</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>292</v>
@@ -7894,7 +7956,7 @@
         <v>483</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E91" s="20" t="s">
         <v>293</v>
@@ -7951,7 +8013,7 @@
         <v>483</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E92" s="14" t="s">
         <v>171</v>
@@ -8008,7 +8070,7 @@
         <v>483</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E93" s="14" t="s">
         <v>289</v>
@@ -8065,7 +8127,7 @@
         <v>483</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E94" s="14" t="s">
         <v>170</v>
@@ -8122,7 +8184,7 @@
         <v>483</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E95" s="24" t="s">
         <v>176</v>
@@ -8179,7 +8241,7 @@
         <v>483</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E96" s="24" t="s">
         <v>369</v>
@@ -8236,7 +8298,7 @@
         <v>483</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E97" s="24" t="s">
         <v>370</v>
@@ -8293,7 +8355,7 @@
         <v>483</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E98" s="24" t="s">
         <v>371</v>
@@ -8350,7 +8412,7 @@
         <v>483</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E99" s="24" t="s">
         <v>384</v>
@@ -8407,7 +8469,7 @@
         <v>483</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E100" s="24" t="s">
         <v>386</v>
@@ -8455,7 +8517,7 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="23" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>473</v>
@@ -8464,10 +8526,10 @@
         <v>483</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E101" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F101" s="24" t="s">
         <v>487</v>
@@ -8523,7 +8585,7 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B102" s="3" t="s">
         <v>473</v>
@@ -8532,10 +8594,10 @@
         <v>483</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E102" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F102" s="24" t="s">
         <v>487</v>
@@ -8591,7 +8653,7 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B103" s="3" t="s">
         <v>473</v>
@@ -8600,10 +8662,10 @@
         <v>483</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E103" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F103" s="24" t="s">
         <v>487</v>
@@ -8659,7 +8721,7 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>473</v>
@@ -8668,10 +8730,10 @@
         <v>483</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E104" s="24" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F104" s="24" t="s">
         <v>487</v>
@@ -8736,7 +8798,7 @@
         <v>483</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>388</v>
@@ -8803,7 +8865,7 @@
         <v>483</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E106" s="24" t="s">
         <v>390</v>
@@ -8870,7 +8932,7 @@
         <v>483</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E107" s="24" t="s">
         <v>392</v>
@@ -8937,7 +8999,7 @@
         <v>483</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E108" s="24" t="s">
         <v>394</v>
@@ -9004,7 +9066,7 @@
         <v>483</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E109" s="24" t="s">
         <v>422</v>
@@ -9061,7 +9123,7 @@
         <v>483</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E110" s="24" t="s">
         <v>424</v>
@@ -9118,7 +9180,7 @@
         <v>483</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>426</v>
@@ -9185,7 +9247,7 @@
         <v>483</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E112" s="24" t="s">
         <v>428</v>
@@ -9242,7 +9304,7 @@
         <v>483</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>430</v>
@@ -9299,7 +9361,7 @@
         <v>483</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E114" s="24" t="s">
         <v>432</v>
@@ -9366,7 +9428,7 @@
         <v>483</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E115" s="24" t="s">
         <v>396</v>
@@ -9423,7 +9485,7 @@
         <v>483</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E116" s="24" t="s">
         <v>398</v>
@@ -9480,7 +9542,7 @@
         <v>483</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E117" s="14" t="s">
         <v>172</v>
@@ -9537,7 +9599,7 @@
         <v>483</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E118" s="14" t="s">
         <v>173</v>
@@ -9594,7 +9656,7 @@
         <v>483</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E119" s="14" t="s">
         <v>174</v>
@@ -9651,7 +9713,7 @@
         <v>483</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E120" s="14" t="s">
         <v>175</v>
@@ -9708,7 +9770,7 @@
         <v>483</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E121" s="14" t="s">
         <v>453</v>
@@ -9765,7 +9827,7 @@
         <v>483</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E122" s="14" t="s">
         <v>455</v>
@@ -9822,7 +9884,7 @@
         <v>483</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E123" s="39" t="s">
         <v>178</v>
@@ -9886,7 +9948,7 @@
         <v>483</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E124" s="39" t="s">
         <v>445</v>
@@ -9954,7 +10016,7 @@
         <v>483</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E125" s="39" t="s">
         <v>449</v>
@@ -10011,7 +10073,7 @@
         <v>483</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E126" s="22" t="s">
         <v>177</v>
@@ -10075,7 +10137,7 @@
         <v>483</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E127" s="22" t="s">
         <v>442</v>
@@ -10132,7 +10194,7 @@
         <v>483</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E128" s="22" t="s">
         <v>311</v>
@@ -10189,7 +10251,7 @@
         <v>483</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E129" s="22" t="s">
         <v>312</v>
@@ -10246,7 +10308,7 @@
         <v>483</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E130" s="22" t="s">
         <v>313</v>
@@ -10303,7 +10365,7 @@
         <v>483</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E131" s="22" t="s">
         <v>314</v>
@@ -10360,7 +10422,7 @@
         <v>483</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E132" s="22" t="s">
         <v>178</v>
@@ -10408,7 +10470,7 @@
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="21" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>473</v>
@@ -10417,7 +10479,7 @@
         <v>483</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E133" s="22" t="s">
         <v>315</v>
@@ -10478,7 +10540,7 @@
         <v>483</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E134" s="22" t="s">
         <v>315</v>
@@ -10535,7 +10597,7 @@
         <v>483</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E135" s="22" t="s">
         <v>316</v>
@@ -10592,7 +10654,7 @@
         <v>483</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E136" s="22" t="s">
         <v>317</v>
@@ -10649,7 +10711,7 @@
         <v>483</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E137" s="22" t="s">
         <v>318</v>
@@ -10706,7 +10768,7 @@
         <v>483</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E138" s="22" t="s">
         <v>180</v>
@@ -10763,7 +10825,7 @@
         <v>483</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E139" s="41" t="s">
         <v>181</v>
@@ -10820,7 +10882,7 @@
         <v>483</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E140" s="24" t="s">
         <v>167</v>
@@ -10877,7 +10939,7 @@
         <v>483</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E141" s="24" t="s">
         <v>168</v>
@@ -10934,7 +10996,7 @@
         <v>483</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E142" s="24" t="s">
         <v>169</v>
@@ -10991,7 +11053,7 @@
         <v>483</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E143" s="24" t="s">
         <v>183</v>
@@ -11048,7 +11110,7 @@
         <v>483</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E144" s="24" t="s">
         <v>303</v>
@@ -11105,7 +11167,7 @@
         <v>483</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E145" s="24" t="s">
         <v>304</v>
@@ -11162,7 +11224,7 @@
         <v>483</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E146" s="24" t="s">
         <v>305</v>
@@ -11219,7 +11281,7 @@
         <v>483</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E147" s="24" t="s">
         <v>306</v>
@@ -11276,7 +11338,7 @@
         <v>483</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E148" s="24" t="s">
         <v>184</v>
@@ -11333,7 +11395,7 @@
         <v>483</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E149" s="14" t="s">
         <v>186</v>
@@ -11390,7 +11452,7 @@
         <v>483</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E150" s="14" t="s">
         <v>307</v>
@@ -11447,7 +11509,7 @@
         <v>483</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E151" s="14" t="s">
         <v>308</v>
@@ -11504,7 +11566,7 @@
         <v>483</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E152" s="14" t="s">
         <v>309</v>
@@ -11561,7 +11623,7 @@
         <v>483</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>310</v>
@@ -11618,7 +11680,7 @@
         <v>483</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>185</v>
@@ -11675,7 +11737,7 @@
         <v>483</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E155" s="10" t="s">
         <v>187</v>
@@ -11732,7 +11794,7 @@
         <v>483</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E156" s="10" t="s">
         <v>298</v>
@@ -11789,7 +11851,7 @@
         <v>483</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E157" s="10" t="s">
         <v>299</v>
@@ -11846,7 +11908,7 @@
         <v>483</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E158" s="10" t="s">
         <v>300</v>
@@ -11903,7 +11965,7 @@
         <v>483</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>302</v>
@@ -11960,7 +12022,7 @@
         <v>483</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>188</v>
@@ -12017,7 +12079,7 @@
         <v>483</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E161" s="26" t="s">
         <v>189</v>
@@ -12073,7 +12135,7 @@
         <v>483</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E162" s="26" t="s">
         <v>319</v>
@@ -12130,7 +12192,7 @@
         <v>483</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E163" s="26" t="s">
         <v>320</v>
@@ -12187,7 +12249,7 @@
         <v>483</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E164" s="26" t="s">
         <v>321</v>
@@ -12244,7 +12306,7 @@
         <v>483</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E165" s="26" t="s">
         <v>322</v>
@@ -12301,7 +12363,7 @@
         <v>483</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E166" s="26" t="s">
         <v>190</v>
@@ -12358,7 +12420,7 @@
         <v>483</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E167" s="32" t="s">
         <v>191</v>
@@ -12415,7 +12477,7 @@
         <v>483</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E168" s="32" t="s">
         <v>323</v>
@@ -12472,7 +12534,7 @@
         <v>483</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E169" s="32" t="s">
         <v>324</v>
@@ -12529,7 +12591,7 @@
         <v>483</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E170" s="32" t="s">
         <v>325</v>
@@ -12586,7 +12648,7 @@
         <v>483</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E171" s="32" t="s">
         <v>326</v>
@@ -12643,7 +12705,7 @@
         <v>483</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E172" s="32" t="s">
         <v>192</v>
@@ -12700,7 +12762,7 @@
         <v>483</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E173" s="12" t="s">
         <v>327</v>
@@ -12757,7 +12819,7 @@
         <v>483</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E174" s="12" t="s">
         <v>329</v>
@@ -12814,7 +12876,7 @@
         <v>483</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E175" s="12" t="s">
         <v>330</v>
@@ -12871,7 +12933,7 @@
         <v>483</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E176" s="12" t="s">
         <v>331</v>
@@ -12928,7 +12990,7 @@
         <v>483</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E177" s="12" t="s">
         <v>332</v>
@@ -12985,7 +13047,7 @@
         <v>483</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E178" s="12" t="s">
         <v>349</v>
@@ -13042,7 +13104,7 @@
         <v>483</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E179" s="12" t="s">
         <v>350</v>
@@ -13099,7 +13161,7 @@
         <v>483</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E180" s="28" t="s">
         <v>351</v>
@@ -13156,7 +13218,7 @@
         <v>483</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E181" s="28" t="s">
         <v>333</v>
@@ -13213,7 +13275,7 @@
         <v>483</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E182" s="28" t="s">
         <v>334</v>
@@ -13270,7 +13332,7 @@
         <v>483</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E183" s="28" t="s">
         <v>335</v>
@@ -13327,7 +13389,7 @@
         <v>483</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>336</v>
@@ -13384,7 +13446,7 @@
         <v>483</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>353</v>
@@ -13441,7 +13503,7 @@
         <v>483</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E186" s="24" t="s">
         <v>193</v>
@@ -13498,7 +13560,7 @@
         <v>483</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E187" s="24" t="s">
         <v>337</v>
@@ -13555,7 +13617,7 @@
         <v>483</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E188" s="24" t="s">
         <v>338</v>
@@ -13612,7 +13674,7 @@
         <v>483</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E189" s="24" t="s">
         <v>339</v>
@@ -13669,7 +13731,7 @@
         <v>483</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E190" s="24" t="s">
         <v>340</v>
@@ -13726,7 +13788,7 @@
         <v>483</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E191" s="24" t="s">
         <v>194</v>
@@ -13783,7 +13845,7 @@
         <v>483</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E192" s="8" t="s">
         <v>355</v>
@@ -13840,7 +13902,7 @@
         <v>483</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E193" s="8" t="s">
         <v>341</v>
@@ -13897,7 +13959,7 @@
         <v>483</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E194" s="8" t="s">
         <v>342</v>
@@ -13954,7 +14016,7 @@
         <v>483</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E195" s="8" t="s">
         <v>343</v>
@@ -14011,7 +14073,7 @@
         <v>483</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>344</v>
@@ -14068,7 +14130,7 @@
         <v>483</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>358</v>
@@ -14125,7 +14187,7 @@
         <v>483</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E198" s="30" t="s">
         <v>356</v>
@@ -14182,7 +14244,7 @@
         <v>483</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E199" s="30" t="s">
         <v>345</v>
@@ -14239,7 +14301,7 @@
         <v>483</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E200" s="30" t="s">
         <v>346</v>
@@ -14296,7 +14358,7 @@
         <v>483</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E201" s="30" t="s">
         <v>347</v>
@@ -14353,7 +14415,7 @@
         <v>483</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E202" s="30" t="s">
         <v>348</v>
@@ -14410,7 +14472,7 @@
         <v>483</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E203" s="30" t="s">
         <v>360</v>
@@ -14467,7 +14529,7 @@
         <v>483</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E204" s="49" t="s">
         <v>203</v>
@@ -14515,7 +14577,7 @@
     </row>
     <row r="205" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>488</v>
+        <v>561</v>
       </c>
       <c r="B205" s="3" t="s">
         <v>473</v>
@@ -14524,49 +14586,61 @@
         <v>483</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E205" s="30" t="s">
+        <v>488</v>
+      </c>
+      <c r="F205" s="30" t="s">
         <v>489</v>
       </c>
-      <c r="F205" s="30" t="s">
-        <v>490</v>
-      </c>
       <c r="G205" s="44">
-        <v>0.5</v>
+        <f t="shared" ref="G205:R205" si="22">0.00002 / 14 / 5</f>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="H205" s="44">
-        <v>2.2000000000000002</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="I205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="J205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="K205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="L205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="M205" s="44">
-        <v>0.1</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="N205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="O205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="P205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="Q205" s="44">
-        <v>1.36</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="R205" s="44">
-        <v>0.1</v>
+        <f t="shared" si="22"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="S205" s="1"/>
       <c r="T205" s="1"/>
@@ -14579,7 +14653,7 @@
     </row>
     <row r="206" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>491</v>
+        <v>562</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>473</v>
@@ -14588,49 +14662,49 @@
         <v>483</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E206" s="30" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F206" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G206" s="44">
-        <v>-100000</v>
+        <v>0.3</v>
       </c>
       <c r="H206" s="44">
-        <v>-100000</v>
+        <v>0.3</v>
       </c>
       <c r="I206" s="44">
-        <v>-30000</v>
+        <v>0.3</v>
       </c>
       <c r="J206" s="44">
-        <v>-30000</v>
+        <v>1.3</v>
       </c>
       <c r="K206" s="44">
-        <v>-30000</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L206" s="44">
-        <v>-30000</v>
+        <v>3.3</v>
       </c>
       <c r="M206" s="44">
-        <v>-30000</v>
+        <v>4.3</v>
       </c>
       <c r="N206" s="44">
-        <v>-30000</v>
+        <v>5.3</v>
       </c>
       <c r="O206" s="44">
-        <v>-30000</v>
+        <v>6.3</v>
       </c>
       <c r="P206" s="44">
-        <v>-30000</v>
+        <v>7.3</v>
       </c>
       <c r="Q206" s="44">
-        <v>-30000</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="R206" s="44">
-        <v>-30000</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="S206" s="51"/>
       <c r="T206" s="51"/>
@@ -14643,7 +14717,7 @@
     </row>
     <row r="207" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>473</v>
@@ -14652,20 +14726,20 @@
         <v>483</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E207" s="30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F207" s="30" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G207" s="44">
         <v>-100000</v>
       </c>
       <c r="H207" s="44">
-        <f t="shared" ref="H207" si="22">H206</f>
-        <v>-100000</v>
+        <f t="shared" ref="H207" si="23">H206</f>
+        <v>0.3</v>
       </c>
       <c r="I207" s="44">
         <v>-100000</v>
@@ -14708,7 +14782,7 @@
     </row>
     <row r="208" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>496</v>
+        <v>563</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>473</v>
@@ -14717,49 +14791,61 @@
         <v>483</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E208" s="50" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F208" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="G208" s="44">
-        <v>0.5</v>
+        <f t="shared" ref="G208:R208" si="24">0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="H208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="I208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="J208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="K208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="L208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="M208" s="44">
-        <v>1</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="N208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="O208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="P208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="Q208" s="44">
-        <v>0.5</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="R208" s="44">
-        <v>1</v>
+        <f t="shared" si="24"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="S208" s="52"/>
       <c r="T208" s="37"/>
@@ -14770,9 +14856,9 @@
       <c r="Y208" s="37"/>
       <c r="Z208" s="37"/>
     </row>
-    <row r="209" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>473</v>
@@ -14781,13 +14867,13 @@
         <v>483</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E209" s="50" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F209" s="50" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G209" s="44" t="s">
         <v>485</v>
@@ -14834,9 +14920,9 @@
       <c r="Y209" s="37"/>
       <c r="Z209" s="37"/>
     </row>
-    <row r="210" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>473</v>
@@ -14845,13 +14931,13 @@
         <v>483</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E210" s="50" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F210" s="50" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G210" s="44">
         <v>0</v>
@@ -14898,9 +14984,9 @@
       <c r="Y210" s="37"/>
       <c r="Z210" s="37"/>
     </row>
-    <row r="211" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>473</v>
@@ -14909,13 +14995,13 @@
         <v>483</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E211" s="50" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F211" s="50" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G211" s="44">
         <v>1E-3</v>
@@ -14962,9 +15048,9 @@
       <c r="Y211" s="37"/>
       <c r="Z211" s="37"/>
     </row>
-    <row r="212" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>473</v>
@@ -14973,10 +15059,10 @@
         <v>483</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E212" s="50" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F212" s="50" t="s">
         <v>487</v>
@@ -15026,9 +15112,9 @@
       <c r="Y212" s="1"/>
       <c r="Z212" s="1"/>
     </row>
-    <row r="213" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>473</v>
@@ -15037,60 +15123,60 @@
         <v>483</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E213" s="50" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F213" s="50" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="G213" s="44">
         <f>1.25*0.000001</f>
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H213" s="44">
-        <f t="shared" ref="H213:R213" si="23">1250*0.000001/5</f>
+        <f t="shared" ref="H213:R213" si="25">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="J213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R213" s="44">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S213" s="51"/>
@@ -15102,9 +15188,9 @@
       <c r="Y213" s="51"/>
       <c r="Z213" s="51"/>
     </row>
-    <row r="214" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>473</v>
@@ -15113,13 +15199,13 @@
         <v>483</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E214" s="50" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F214" s="50" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G214" s="44">
         <v>2.0000000000000001E-4</v>
@@ -15166,9 +15252,9 @@
       <c r="Y214" s="51"/>
       <c r="Z214" s="51"/>
     </row>
-    <row r="215" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>473</v>
@@ -15177,13 +15263,13 @@
         <v>483</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E215" s="50" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F215" s="50" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G215" s="44">
         <v>2.4999999999999998E-12</v>
@@ -15230,9 +15316,9 @@
       <c r="Y215" s="51"/>
       <c r="Z215" s="51"/>
     </row>
-    <row r="216" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>473</v>
@@ -15241,13 +15327,13 @@
         <v>483</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E216" s="50" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F216" s="50" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G216" s="44">
         <v>1.2E-8</v>
@@ -15256,7 +15342,8 @@
         <v>1.2E-8</v>
       </c>
       <c r="I216" s="44">
-        <v>1.1999999999999999E-7</v>
+        <f>0.00000012*100</f>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="J216" s="44">
         <v>1.1999999999999999E-7</v>
@@ -15294,9 +15381,9 @@
       <c r="Y216" s="51"/>
       <c r="Z216" s="51"/>
     </row>
-    <row r="217" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>473</v>
@@ -15305,13 +15392,13 @@
         <v>483</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E217" s="50" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F217" s="50" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="G217" s="44">
         <v>9.9999999999999995E-8</v>
@@ -15358,9 +15445,9 @@
       <c r="Y217" s="51"/>
       <c r="Z217" s="51"/>
     </row>
-    <row r="218" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>473</v>
@@ -15369,13 +15456,13 @@
         <v>483</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E218" s="50" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F218" s="50" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="G218" s="44">
         <f>2*0.00001</f>
@@ -15424,9 +15511,9 @@
       <c r="Y218" s="51"/>
       <c r="Z218" s="51"/>
     </row>
-    <row r="219" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>473</v>
@@ -15435,13 +15522,13 @@
         <v>483</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E219" s="50" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F219" s="50" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="G219" s="44">
         <f>0.00000000000001 * 1000</f>
@@ -15452,43 +15539,43 @@
         <v>9.9999999999999994E-12</v>
       </c>
       <c r="I219" s="44">
-        <f t="shared" ref="I219:R219" si="24">0.00000000000001*10000*8</f>
+        <f t="shared" ref="I219:R219" si="26">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="J219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="K219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="L219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="M219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="N219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="O219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="P219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Q219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="R219" s="44">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="S219" s="51"/>
@@ -15500,9 +15587,9 @@
       <c r="Y219" s="51"/>
       <c r="Z219" s="51"/>
     </row>
-    <row r="220" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>473</v>
@@ -15511,13 +15598,13 @@
         <v>483</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E220" s="50" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F220" s="50" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="G220" s="44">
         <f>0.00000000000001 * 10000</f>
@@ -15528,43 +15615,43 @@
         <v>1E-10</v>
       </c>
       <c r="I220" s="44">
-        <f t="shared" ref="I220:J220" si="25">I219*10</f>
+        <f t="shared" ref="I220:J220" si="27">I219*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="J220" s="44">
-        <f t="shared" si="25"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="K220" s="44">
-        <f t="shared" ref="K220:L220" si="26">K219*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="L220" s="44">
-        <f t="shared" si="26"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="M220" s="44">
-        <f t="shared" ref="M220:N220" si="27">M219*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="N220" s="44">
         <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="O220" s="44">
-        <f t="shared" ref="O220:P220" si="28">O219*10</f>
+      <c r="K220" s="44">
+        <f t="shared" ref="K220:L220" si="28">K219*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="P220" s="44">
+      <c r="L220" s="44">
         <f t="shared" si="28"/>
         <v>8.0000000000000005E-9</v>
       </c>
+      <c r="M220" s="44">
+        <f t="shared" ref="M220:N220" si="29">M219*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="N220" s="44">
+        <f t="shared" si="29"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="O220" s="44">
+        <f t="shared" ref="O220:P220" si="30">O219*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="P220" s="44">
+        <f t="shared" si="30"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
       <c r="Q220" s="44">
-        <f t="shared" ref="Q220:R220" si="29">Q219*10</f>
+        <f t="shared" ref="Q220:R220" si="31">Q219*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="R220" s="44">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="S220" s="51"/>
@@ -15576,7 +15663,7 @@
       <c r="Y220" s="51"/>
       <c r="Z220" s="51"/>
     </row>
-    <row r="221" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>486</v>
       </c>
@@ -15587,60 +15674,60 @@
         <v>483</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E221" s="50" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F221" s="50" t="s">
         <v>487</v>
       </c>
       <c r="G221" s="44">
-        <f t="shared" ref="G221:R221" si="30">0.84*(0.36^2)</f>
+        <f t="shared" ref="G221:R221" si="32">0.84*(0.36^2)</f>
         <v>0.10886399999999999</v>
       </c>
       <c r="H221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="I221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="J221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="K221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="L221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="M221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="N221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="O221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="P221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="Q221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="R221" s="44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.10886399999999999</v>
       </c>
       <c r="S221" s="51"/>
@@ -15652,24 +15739,24 @@
       <c r="Y221" s="51"/>
       <c r="Z221" s="51"/>
     </row>
-    <row r="222" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>473</v>
       </c>
       <c r="C222" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="D222" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="D222" s="3" t="s">
-        <v>542</v>
-      </c>
       <c r="E222" s="50" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F222" s="50" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="G222" s="44">
         <v>9.9999999999999995E-8</v>
@@ -15681,42 +15768,449 @@
       <c r="I222" s="44">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="J222" s="44">
+      <c r="J222" s="57">
         <f>0.0000001</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="K222" s="44">
+      <c r="K222" s="57">
         <f>0.0000001*2</f>
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="L222" s="44">
+      <c r="L222" s="57">
         <f>0.0000001*3</f>
         <v>2.9999999999999999E-7</v>
       </c>
-      <c r="M222" s="44">
+      <c r="M222" s="57">
         <f>0.0000001</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="N222" s="44">
+      <c r="N222" s="57">
         <f>0.0000001*6</f>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="O222" s="44">
+      <c r="O222" s="57">
         <f>0.0000001*6</f>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="P222" s="44">
+      <c r="P222" s="57">
         <f>0.0000001*6</f>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="Q222" s="44">
+      <c r="Q222" s="57">
         <f>0.0000001*10</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="R222" s="44">
+      <c r="R222" s="57">
         <f>0.0000001*10*2</f>
         <v>1.9999999999999999E-6</v>
       </c>
+    </row>
+    <row r="223" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A223" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E223" s="50" t="s">
+        <v>552</v>
+      </c>
+      <c r="F223" s="50" t="s">
+        <v>489</v>
+      </c>
+      <c r="G223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="H223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="I223" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="J223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="K223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="L223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="M223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="N223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="O223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="P223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="Q223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="R223" s="52">
+        <v>0.2</v>
+      </c>
+      <c r="S223" s="58"/>
+      <c r="T223" s="58"/>
+      <c r="U223" s="58"/>
+      <c r="V223" s="58"/>
+      <c r="W223" s="58"/>
+      <c r="X223" s="58"/>
+      <c r="Y223" s="58"/>
+      <c r="Z223" s="58"/>
+      <c r="AA223" s="58"/>
+      <c r="AB223" s="58"/>
+      <c r="AC223" s="58"/>
+      <c r="AD223" s="58"/>
+      <c r="AE223" s="58"/>
+      <c r="AF223" s="58"/>
+      <c r="AG223" s="58"/>
+      <c r="AH223" s="58"/>
+      <c r="AI223" s="58"/>
+      <c r="AJ223" s="58"/>
+      <c r="AK223" s="58"/>
+      <c r="AL223" s="58"/>
+      <c r="AM223" s="58"/>
+      <c r="AN223" s="58"/>
+      <c r="AO223" s="58"/>
+    </row>
+    <row r="224" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A224" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E224" s="50" t="s">
+        <v>554</v>
+      </c>
+      <c r="F224" s="50" t="s">
+        <v>497</v>
+      </c>
+      <c r="G224" s="52" t="s">
+        <v>485</v>
+      </c>
+      <c r="H224" s="52" t="s">
+        <v>485</v>
+      </c>
+      <c r="I224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="J224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="K224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="L224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="M224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="N224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="O224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="P224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="R224" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="S224" s="58"/>
+      <c r="T224" s="58"/>
+      <c r="U224" s="58"/>
+      <c r="V224" s="58"/>
+      <c r="W224" s="58"/>
+      <c r="X224" s="58"/>
+      <c r="Y224" s="58"/>
+      <c r="Z224" s="58"/>
+      <c r="AA224" s="58"/>
+      <c r="AB224" s="58"/>
+      <c r="AC224" s="58"/>
+      <c r="AD224" s="58"/>
+      <c r="AE224" s="58"/>
+      <c r="AF224" s="58"/>
+      <c r="AG224" s="58"/>
+      <c r="AH224" s="58"/>
+      <c r="AI224" s="58"/>
+      <c r="AJ224" s="58"/>
+      <c r="AK224" s="58"/>
+      <c r="AL224" s="58"/>
+      <c r="AM224" s="58"/>
+      <c r="AN224" s="58"/>
+      <c r="AO224" s="58"/>
+    </row>
+    <row r="225" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A225" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E225" s="50" t="s">
+        <v>556</v>
+      </c>
+      <c r="F225" s="50" t="s">
+        <v>497</v>
+      </c>
+      <c r="G225" s="52">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="H225" s="52">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="I225" s="55">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="J225" s="55">
+        <f t="shared" ref="J225:R225" si="33">2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="K225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="L225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="M225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="N225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="O225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="P225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="Q225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="R225" s="55">
+        <f t="shared" si="33"/>
+        <v>0.2</v>
+      </c>
+      <c r="S225" s="58"/>
+      <c r="T225" s="58"/>
+      <c r="U225" s="58"/>
+      <c r="V225" s="58"/>
+      <c r="W225" s="58"/>
+      <c r="X225" s="58"/>
+      <c r="Y225" s="58"/>
+      <c r="Z225" s="58"/>
+      <c r="AA225" s="58"/>
+      <c r="AB225" s="58"/>
+      <c r="AC225" s="58"/>
+      <c r="AD225" s="58"/>
+      <c r="AE225" s="58"/>
+      <c r="AF225" s="58"/>
+      <c r="AG225" s="58"/>
+      <c r="AH225" s="58"/>
+      <c r="AI225" s="58"/>
+      <c r="AJ225" s="58"/>
+      <c r="AK225" s="58"/>
+      <c r="AL225" s="58"/>
+      <c r="AM225" s="58"/>
+      <c r="AN225" s="58"/>
+      <c r="AO225" s="58"/>
+    </row>
+    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E226" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="F226" s="50" t="s">
+        <v>497</v>
+      </c>
+      <c r="G226" s="52">
+        <v>1E-3</v>
+      </c>
+      <c r="H226" s="52">
+        <v>1E-3</v>
+      </c>
+      <c r="I226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="J226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="K226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="L226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="M226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="N226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="O226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="P226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="Q226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="R226" s="55">
+        <v>1E-3</v>
+      </c>
+      <c r="S226" s="58"/>
+      <c r="T226" s="58"/>
+      <c r="U226" s="58"/>
+      <c r="V226" s="58"/>
+      <c r="W226" s="58"/>
+      <c r="X226" s="58"/>
+      <c r="Y226" s="58"/>
+      <c r="Z226" s="58"/>
+      <c r="AA226" s="58"/>
+      <c r="AB226" s="58"/>
+      <c r="AC226" s="58"/>
+      <c r="AD226" s="58"/>
+      <c r="AE226" s="58"/>
+      <c r="AF226" s="58"/>
+      <c r="AG226" s="58"/>
+      <c r="AH226" s="58"/>
+      <c r="AI226" s="58"/>
+      <c r="AJ226" s="58"/>
+      <c r="AK226" s="58"/>
+      <c r="AL226" s="58"/>
+      <c r="AM226" s="58"/>
+      <c r="AN226" s="58"/>
+      <c r="AO226" s="58"/>
+    </row>
+    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="E227" s="50" t="s">
+        <v>560</v>
+      </c>
+      <c r="F227" s="50" t="s">
+        <v>497</v>
+      </c>
+      <c r="G227" s="53">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H227" s="53">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="M227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="N227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="O227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Q227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="R227" s="56">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="S227" s="59"/>
+      <c r="T227" s="59"/>
+      <c r="U227" s="59"/>
+      <c r="V227" s="59"/>
+      <c r="W227" s="59"/>
+      <c r="X227" s="59"/>
+      <c r="Y227" s="59"/>
+      <c r="Z227" s="59"/>
+      <c r="AA227" s="59"/>
+      <c r="AB227" s="59"/>
+      <c r="AC227" s="59"/>
+      <c r="AD227" s="54"/>
+      <c r="AE227" s="59"/>
+      <c r="AF227" s="59"/>
+      <c r="AG227" s="59"/>
+      <c r="AH227" s="59"/>
+      <c r="AI227" s="59"/>
+      <c r="AJ227" s="59"/>
+      <c r="AK227" s="59"/>
+      <c r="AL227" s="59"/>
+      <c r="AM227" s="59"/>
+      <c r="AN227" s="59"/>
+      <c r="AO227" s="59"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:R2">
@@ -20575,7 +21069,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>

</xml_diff>